<commit_message>
WORKS third algorithm (IT_SORAN testing)
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/EdgeSignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/EdgeSignalConfigs/SignalConfigs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\EdgeSignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B644967E-E4C0-4546-BFD3-EC2D27AB1F0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98B1555-8737-46F6-8A63-1C9D27B22B5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Config Name</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Testt</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Fast</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,6 +484,64 @@
         <v>0.45</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
sending is ready for testing in IT_SORAN
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/EdgeSignalConfigs/SignalConfigs.xlsx
+++ b/SignalGenerationConfigs/EdgeSignalConfigs/SignalConfigs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\SignalGenerationConfigs\EdgeSignalConfigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220EAB3D-F5D2-49DC-931B-8BB8B39282EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E86CF5-2ED0-4AF0-8C0F-BB210F64D5E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Config Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Request Frequency</t>
   </si>
   <si>
-    <t>Testt</t>
-  </si>
-  <si>
     <t>Slow</t>
   </si>
   <si>
@@ -59,6 +56,15 @@
   </si>
   <si>
     <t>Debug</t>
+  </si>
+  <si>
+    <t>TestAcc</t>
+  </si>
+  <si>
+    <t>TestDec</t>
+  </si>
+  <si>
+    <t>TimeTest</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,38 +464,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>0.45</v>
-      </c>
-    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -518,7 +495,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -547,7 +524,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -572,6 +549,93 @@
       </c>
       <c r="I5">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>